<commit_message>
Refactor the code structure: Abstacted Clusters to another folder Abstracted Models to another folder Parallel and Serial algorithms in seperate folder Core functionalities and add-ons are in Core/  folder README updated. New algorithms: Quasi-Collapsed and P-Quasi Collapsed Quasi-Direct and P-Quasi-Direct Bug Fixes: Direct Gibbs weight sampling New conjugates Dirichlet-Multinomial for discrete data Documentation tex updated
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="alldata" sheetId="1" r:id="rId1"/>
-    <sheet name="directexperiments" sheetId="2" r:id="rId2"/>
+    <sheet name="q-directexperiments" sheetId="2" r:id="rId2"/>
     <sheet name="collapsedexperiments" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -49,12 +49,6 @@
     <t>𝛼</t>
   </si>
   <si>
-    <t>P-Direct</t>
-  </si>
-  <si>
-    <t>Direct</t>
-  </si>
-  <si>
     <t>Collapsed</t>
   </si>
   <si>
@@ -80,6 +74,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>P-Q-Direct</t>
+  </si>
+  <si>
+    <t>Q-Direct</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>P-Direct</c:v>
+                  <c:v>P-Q-Direct</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -792,11 +792,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-9669200"/>
-        <c:axId val="-213632960"/>
+        <c:axId val="1842050896"/>
+        <c:axId val="1842054800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-9669200"/>
+        <c:axId val="1842050896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -895,7 +895,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-213632960"/>
+        <c:crossAx val="1842054800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -903,7 +903,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-213632960"/>
+        <c:axId val="1842054800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1010,7 +1010,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-9669200"/>
+        <c:crossAx val="1842050896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1183,7 +1183,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>P-Direct</c:v>
+                  <c:v>P-Q-Direct</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1624,11 +1624,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-26206272"/>
-        <c:axId val="-213831664"/>
+        <c:axId val="1843632528"/>
+        <c:axId val="1843496656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-26206272"/>
+        <c:axId val="1843632528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,7 +1727,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-213831664"/>
+        <c:crossAx val="1843496656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1735,7 +1735,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-213831664"/>
+        <c:axId val="1843496656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1841,7 +1841,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-26206272"/>
+        <c:crossAx val="1843632528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2014,7 +2014,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>P-Direct</c:v>
+                  <c:v>P-Q-Direct</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2455,11 +2455,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-26825776"/>
-        <c:axId val="-27146592"/>
+        <c:axId val="1843421408"/>
+        <c:axId val="1842063296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-26825776"/>
+        <c:axId val="1843421408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2558,7 +2558,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-27146592"/>
+        <c:crossAx val="1842063296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2566,7 +2566,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-27146592"/>
+        <c:axId val="1842063296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2672,7 +2672,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-26825776"/>
+        <c:crossAx val="1843421408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2845,7 +2845,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>P-Direct</c:v>
+                  <c:v>P-Q-Direct</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3286,11 +3286,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-9667184"/>
-        <c:axId val="-26623536"/>
+        <c:axId val="1842101856"/>
+        <c:axId val="1842105760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-9667184"/>
+        <c:axId val="1842101856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3389,7 +3389,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-26623536"/>
+        <c:crossAx val="1842105760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3397,7 +3397,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-26623536"/>
+        <c:axId val="1842105760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3504,7 +3504,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-9667184"/>
+        <c:crossAx val="1842101856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5913,8 +5913,8 @@
     <tableColumn id="3" name="Kinit" dataDxfId="5"/>
     <tableColumn id="4" name="𝛼" dataDxfId="4"/>
     <tableColumn id="9" name="D" dataDxfId="3"/>
-    <tableColumn id="5" name="P-Direct" dataDxfId="2"/>
-    <tableColumn id="6" name="Direct" dataDxfId="1"/>
+    <tableColumn id="5" name="P-Q-Direct" dataDxfId="2"/>
+    <tableColumn id="6" name="Q-Direct" dataDxfId="1"/>
     <tableColumn id="7" name="Collapsed" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6207,8 +6207,8 @@
   </sheetPr>
   <dimension ref="A1:H192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="H183" sqref="H183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6231,16 +6231,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -10925,7 +10925,7 @@
     </row>
     <row r="192" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E192" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -15105,22 +15105,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>